<commit_message>
Added fuel demand as possible constraint
</commit_message>
<xml_diff>
--- a/Fuels_case_input_test_190827.xlsx
+++ b/Fuels_case_input_test_190827.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/IDrive-Sync/Carnegie/SEM-1.2_CIW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010E2698-0A04-D746-B765-61145FB04883}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA6EF21-FAB7-F846-8051-47F171EAA73F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10500" yWindow="-28160" windowWidth="49300" windowHeight="26420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_test_190726" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="214">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -661,9 +661,6 @@
     <t>Input_Data/SEM_TEMOA</t>
   </si>
   <si>
-    <t>test_190829_v5</t>
-  </si>
-  <si>
     <t>SEM_TEMOA_demand.csv</t>
   </si>
   <si>
@@ -671,6 +668,15 @@
   </si>
   <si>
     <t>SEM_TEMOA_wind.csv</t>
+  </si>
+  <si>
+    <t>FUEL_DEMAND</t>
+  </si>
+  <si>
+    <t>MWh</t>
+  </si>
+  <si>
+    <t>test_190829_v6</t>
   </si>
 </sst>
 </file>
@@ -823,7 +829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1017,6 +1023,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1332,14 +1339,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR1029"/>
+  <dimension ref="A1:AS1030"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5480" ySplit="5320" topLeftCell="A83" activePane="bottomRight"/>
+      <pane xSplit="5480" ySplit="5320" topLeftCell="A42" activePane="bottomRight"/>
       <selection activeCell="A62" sqref="A62:XFD62"/>
       <selection pane="topRight" activeCell="F81" sqref="F81"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A62:XFD80"/>
-      <selection pane="bottomRight" activeCell="B90" sqref="B90"/>
+      <selection pane="bottomLeft" activeCell="C159" sqref="C159"/>
+      <selection pane="bottomRight" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3056,7 +3063,7 @@
         <v>33</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>34</v>
@@ -3559,7 +3566,7 @@
         <v>76</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="4"/>
@@ -4059,7 +4066,7 @@
         <v>91</v>
       </c>
       <c r="B80" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="4"/>
@@ -4335,7 +4342,7 @@
         <v>167</v>
       </c>
       <c r="B86" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="4"/>
@@ -4611,7 +4618,7 @@
         <v>104</v>
       </c>
       <c r="B92" s="50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
@@ -4887,7 +4894,7 @@
         <v>172</v>
       </c>
       <c r="B98" s="50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
@@ -6927,7 +6934,7 @@
         <v>157</v>
       </c>
       <c r="B141" s="47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F141" s="8"/>
       <c r="H141" s="8"/>
@@ -7601,8 +7608,17 @@
       <c r="Z158" s="20"/>
     </row>
     <row r="159" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="52"/>
-      <c r="B159" s="47"/>
+      <c r="A159" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="B159" s="49">
+        <v>1</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D159" s="69"/>
+      <c r="E159" s="3"/>
       <c r="F159" s="8"/>
       <c r="H159" s="8"/>
       <c r="I159" s="3"/>
@@ -7648,20 +7664,10 @@
       <c r="Y160" s="25"/>
       <c r="Z160" s="20"/>
     </row>
-    <row r="161" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B161" s="15">
-        <v>10</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D161" s="3"/>
-      <c r="E161" s="4"/>
+    <row r="161" spans="1:45" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="52"/>
+      <c r="B161" s="47"/>
       <c r="F161" s="8"/>
-      <c r="G161" s="3"/>
       <c r="H161" s="8"/>
       <c r="I161" s="3"/>
       <c r="J161" s="18"/>
@@ -7681,47 +7687,48 @@
       <c r="X161" s="24"/>
       <c r="Y161" s="25"/>
       <c r="Z161" s="20"/>
-      <c r="AA161" s="4"/>
-      <c r="AB161" s="4"/>
-      <c r="AC161" s="4"/>
-    </row>
-    <row r="162" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="3"/>
-      <c r="B162" s="4"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="4"/>
-      <c r="E162" s="3"/>
-      <c r="F162" s="4"/>
+    </row>
+    <row r="162" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B162" s="15">
+        <v>10</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D162" s="3"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="8"/>
       <c r="G162" s="3"/>
-      <c r="H162" s="4"/>
-      <c r="I162" s="4"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
+      <c r="H162" s="8"/>
+      <c r="I162" s="3"/>
+      <c r="J162" s="18"/>
+      <c r="K162" s="8"/>
       <c r="L162" s="4"/>
-      <c r="M162" s="4"/>
-      <c r="N162" s="4"/>
-      <c r="O162" s="4"/>
-      <c r="P162" s="4"/>
-      <c r="Q162" s="4"/>
+      <c r="M162" s="18"/>
+      <c r="N162" s="20"/>
+      <c r="O162" s="8"/>
+      <c r="P162" s="8"/>
+      <c r="Q162" s="21"/>
       <c r="R162" s="4"/>
-      <c r="S162" s="4"/>
+      <c r="S162" s="8"/>
       <c r="T162" s="4"/>
-      <c r="U162" s="4"/>
-      <c r="V162" s="4"/>
-      <c r="W162" s="4"/>
-      <c r="X162" s="4"/>
-      <c r="Y162" s="4"/>
-      <c r="Z162" s="4"/>
+      <c r="U162" s="22"/>
+      <c r="V162" s="22"/>
+      <c r="W162" s="23"/>
+      <c r="X162" s="24"/>
+      <c r="Y162" s="25"/>
+      <c r="Z162" s="20"/>
       <c r="AA162" s="4"/>
       <c r="AB162" s="4"/>
       <c r="AC162" s="4"/>
     </row>
-    <row r="163" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3"/>
       <c r="B163" s="4"/>
-      <c r="C163" s="3" t="s">
-        <v>146</v>
-      </c>
+      <c r="C163" s="3"/>
       <c r="D163" s="4"/>
       <c r="E163" s="3"/>
       <c r="F163" s="4"/>
@@ -7749,10 +7756,12 @@
       <c r="AB163" s="4"/>
       <c r="AC163" s="4"/>
     </row>
-    <row r="164" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3"/>
       <c r="B164" s="4"/>
-      <c r="C164" s="3"/>
+      <c r="C164" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="D164" s="4"/>
       <c r="E164" s="3"/>
       <c r="F164" s="4"/>
@@ -7780,365 +7789,371 @@
       <c r="AB164" s="4"/>
       <c r="AC164" s="4"/>
     </row>
-    <row r="165" spans="1:44" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="54" t="s">
+    <row r="165" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="3"/>
+      <c r="B165" s="4"/>
+      <c r="C165" s="3"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="3"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="3"/>
+      <c r="H165" s="4"/>
+      <c r="I165" s="4"/>
+      <c r="J165" s="4"/>
+      <c r="K165" s="4"/>
+      <c r="L165" s="4"/>
+      <c r="M165" s="4"/>
+      <c r="N165" s="4"/>
+      <c r="O165" s="4"/>
+      <c r="P165" s="4"/>
+      <c r="Q165" s="4"/>
+      <c r="R165" s="4"/>
+      <c r="S165" s="4"/>
+      <c r="T165" s="4"/>
+      <c r="U165" s="4"/>
+      <c r="V165" s="4"/>
+      <c r="W165" s="4"/>
+      <c r="X165" s="4"/>
+      <c r="Y165" s="4"/>
+      <c r="Z165" s="4"/>
+      <c r="AA165" s="4"/>
+      <c r="AB165" s="4"/>
+      <c r="AC165" s="4"/>
+    </row>
+    <row r="166" spans="1:45" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="B165" s="43" t="s">
+      <c r="B166" s="43" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="166" spans="1:44" s="44" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A166" s="44" t="s">
+    <row r="167" spans="1:45" s="44" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A167" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="B166" s="51" t="s">
+      <c r="B167" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="C166" s="51" t="s">
+      <c r="C167" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D166" s="51" t="s">
+      <c r="D167" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="E166" s="51" t="s">
+      <c r="E167" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="F166" s="51" t="s">
+      <c r="F167" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="G166" s="51" t="s">
+      <c r="G167" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="H166" s="51" t="s">
+      <c r="H167" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="I166" s="51" t="s">
+      <c r="I167" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="J166" s="51" t="s">
+      <c r="J167" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="K166" s="51" t="s">
+      <c r="K167" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="L166" s="51" t="s">
+      <c r="L167" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="M166" s="51" t="s">
+      <c r="M167" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="N166" s="51" t="s">
+      <c r="N167" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="O166" s="51" t="s">
+      <c r="O167" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="P166" s="51" t="s">
+      <c r="P167" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="Q166" s="51" t="s">
+      <c r="Q167" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="R166" s="51" t="s">
+      <c r="R167" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="S166" s="51" t="s">
+      <c r="S167" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="T166" s="51" t="s">
+      <c r="T167" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="U166" s="51" t="s">
+      <c r="U167" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="V166" s="51" t="s">
+      <c r="V167" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="W166" s="51" t="s">
+      <c r="W167" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="X166" s="51" t="s">
+      <c r="X167" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="Y166" s="51" t="s">
+      <c r="Y167" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="Z166" s="51" t="s">
+      <c r="Z167" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="AA166" s="51" t="s">
+      <c r="AA167" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="AB166" s="51" t="s">
+      <c r="AB167" s="51" t="s">
         <v>181</v>
       </c>
-      <c r="AC166" s="51" t="s">
+      <c r="AC167" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="AD166" s="51" t="s">
+      <c r="AD167" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="AE166" s="51" t="s">
+      <c r="AE167" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="AF166" s="51" t="s">
+      <c r="AF167" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="AG166" s="51" t="s">
+      <c r="AG167" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="AH166" s="51" t="s">
+      <c r="AH167" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="AI166" s="51" t="s">
+      <c r="AI167" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="AJ166" s="51" t="s">
+      <c r="AJ167" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="AK166" s="51" t="s">
+      <c r="AK167" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="AL166" s="51" t="s">
+      <c r="AL167" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="AM166" s="51" t="s">
+      <c r="AM167" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="AN166" s="51" t="s">
+      <c r="AN167" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="AO166" s="51" t="s">
+      <c r="AO167" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="AP166" s="44" t="s">
+      <c r="AP167" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="AQ166" s="44" t="s">
+      <c r="AQ167" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="AR166" s="44" t="s">
+      <c r="AR167" s="44" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="167" spans="1:44" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B167" s="55"/>
-      <c r="C167" s="55"/>
-      <c r="D167" s="55"/>
-      <c r="E167" s="55"/>
-      <c r="F167" s="55"/>
-      <c r="G167" s="55"/>
-      <c r="H167" s="55"/>
-      <c r="I167" s="55"/>
-      <c r="J167" s="55"/>
-      <c r="K167" s="55"/>
-      <c r="L167" s="55"/>
-      <c r="M167" s="55"/>
-      <c r="N167" s="55"/>
-      <c r="O167" s="55"/>
-      <c r="P167" s="55"/>
-      <c r="Q167" s="55"/>
-      <c r="R167" s="55"/>
-      <c r="S167" s="55"/>
-      <c r="T167" s="55"/>
-      <c r="U167" s="55"/>
-      <c r="V167" s="55"/>
-      <c r="W167" s="55"/>
-      <c r="X167" s="55"/>
-      <c r="Y167" s="55"/>
-      <c r="Z167" s="55"/>
-      <c r="AA167" s="55"/>
-      <c r="AB167" s="55"/>
-      <c r="AC167" s="55"/>
-      <c r="AD167" s="55"/>
-      <c r="AE167" s="55"/>
-      <c r="AF167" s="55"/>
-      <c r="AG167" s="55"/>
-      <c r="AH167" s="55"/>
-      <c r="AI167" s="55"/>
-      <c r="AJ167" s="55"/>
-      <c r="AK167" s="55"/>
-      <c r="AL167" s="55"/>
-      <c r="AM167" s="55"/>
-      <c r="AN167" s="55"/>
-      <c r="AO167" s="55"/>
-    </row>
-    <row r="168" spans="1:44" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="56" t="s">
+      <c r="AS167" s="44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="168" spans="1:45" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B168" s="55"/>
+      <c r="C168" s="55"/>
+      <c r="D168" s="55"/>
+      <c r="E168" s="55"/>
+      <c r="F168" s="55"/>
+      <c r="G168" s="55"/>
+      <c r="H168" s="55"/>
+      <c r="I168" s="55"/>
+      <c r="J168" s="55"/>
+      <c r="K168" s="55"/>
+      <c r="L168" s="55"/>
+      <c r="M168" s="55"/>
+      <c r="N168" s="55"/>
+      <c r="O168" s="55"/>
+      <c r="P168" s="55"/>
+      <c r="Q168" s="55"/>
+      <c r="R168" s="55"/>
+      <c r="S168" s="55"/>
+      <c r="T168" s="55"/>
+      <c r="U168" s="55"/>
+      <c r="V168" s="55"/>
+      <c r="W168" s="55"/>
+      <c r="X168" s="55"/>
+      <c r="Y168" s="55"/>
+      <c r="Z168" s="55"/>
+      <c r="AA168" s="55"/>
+      <c r="AB168" s="55"/>
+      <c r="AC168" s="55"/>
+      <c r="AD168" s="55"/>
+      <c r="AE168" s="55"/>
+      <c r="AF168" s="55"/>
+      <c r="AG168" s="55"/>
+      <c r="AH168" s="55"/>
+      <c r="AI168" s="55"/>
+      <c r="AJ168" s="55"/>
+      <c r="AK168" s="55"/>
+      <c r="AL168" s="55"/>
+      <c r="AM168" s="55"/>
+      <c r="AN168" s="55"/>
+      <c r="AO168" s="55"/>
+    </row>
+    <row r="169" spans="1:45" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="B168" s="57">
+      <c r="B169" s="57">
         <v>2016</v>
       </c>
-      <c r="C168" s="57">
+      <c r="C169" s="57">
         <v>1</v>
       </c>
-      <c r="D168" s="57">
+      <c r="D169" s="57">
         <v>2016</v>
       </c>
-      <c r="E168" s="57">
+      <c r="E169" s="57">
         <v>1</v>
       </c>
-      <c r="F168" s="57">
+      <c r="F169" s="57">
         <v>1</v>
       </c>
-      <c r="G168" s="57">
+      <c r="G169" s="57">
         <v>1</v>
       </c>
-      <c r="H168" s="57">
+      <c r="H169" s="57">
         <v>-1</v>
       </c>
-      <c r="I168" s="57">
+      <c r="I169" s="57">
         <v>1</v>
       </c>
-      <c r="J168" s="57">
+      <c r="J169" s="57">
         <v>1</v>
       </c>
-      <c r="K168" s="57">
+      <c r="K169" s="57">
         <v>1</v>
       </c>
-      <c r="L168" s="57">
+      <c r="L169" s="57">
         <v>-1</v>
       </c>
-      <c r="M168" s="57">
+      <c r="M169" s="57">
         <v>1</v>
       </c>
-      <c r="N168" s="57">
+      <c r="N169" s="57">
         <v>-1</v>
       </c>
-      <c r="O168" s="57">
+      <c r="O169" s="57">
         <v>1</v>
       </c>
-      <c r="P168" s="57">
+      <c r="P169" s="57">
         <v>-1</v>
       </c>
-      <c r="Q168" s="57">
+      <c r="Q169" s="57">
         <v>1</v>
       </c>
-      <c r="R168" s="57">
+      <c r="R169" s="57">
         <v>1</v>
       </c>
-      <c r="S168" s="57">
+      <c r="S169" s="57">
         <v>1</v>
       </c>
-      <c r="T168" s="57">
+      <c r="T169" s="57">
         <v>-1</v>
       </c>
-      <c r="U168" s="57">
+      <c r="U169" s="57">
         <v>-1</v>
       </c>
-      <c r="V168" s="57">
+      <c r="V169" s="57">
         <v>1</v>
       </c>
-      <c r="W168" s="57">
+      <c r="W169" s="57">
         <v>1</v>
       </c>
-      <c r="X168" s="57">
+      <c r="X169" s="57">
         <v>0.9</v>
       </c>
-      <c r="Y168" s="58">
+      <c r="Y169" s="58">
         <v>-1</v>
       </c>
-      <c r="Z168" s="58">
+      <c r="Z169" s="58">
         <v>-1</v>
       </c>
-      <c r="AA168" s="57">
+      <c r="AA169" s="57">
         <v>0.3</v>
       </c>
-      <c r="AB168" s="57">
+      <c r="AB169" s="57">
         <v>0.1</v>
       </c>
-      <c r="AC168" s="57">
+      <c r="AC169" s="57">
         <v>-1</v>
       </c>
-      <c r="AD168" s="58">
+      <c r="AD169" s="58">
         <v>1</v>
       </c>
-      <c r="AE168" s="58">
+      <c r="AE169" s="58">
         <v>1</v>
       </c>
-      <c r="AF168" s="57">
+      <c r="AF169" s="57">
         <v>1</v>
       </c>
-      <c r="AG168" s="57">
+      <c r="AG169" s="57">
         <v>-1</v>
       </c>
-      <c r="AH168" s="57">
+      <c r="AH169" s="57">
         <v>1</v>
       </c>
-      <c r="AI168" s="57">
+      <c r="AI169" s="57">
         <v>-1</v>
       </c>
-      <c r="AJ168" s="57">
+      <c r="AJ169" s="57">
         <v>1</v>
       </c>
-      <c r="AK168" s="57">
+      <c r="AK169" s="57">
         <v>1</v>
       </c>
-      <c r="AL168" s="57">
+      <c r="AL169" s="57">
         <v>1</v>
       </c>
-      <c r="AM168" s="57">
+      <c r="AM169" s="57">
         <v>1</v>
       </c>
-      <c r="AN168" s="57">
+      <c r="AN169" s="57">
         <v>-1</v>
       </c>
-      <c r="AO168" s="57">
+      <c r="AO169" s="57">
         <v>1</v>
       </c>
-      <c r="AP168" s="56">
+      <c r="AP169" s="56">
         <v>1</v>
       </c>
-      <c r="AQ168" s="59">
+      <c r="AQ169" s="59">
         <v>1</v>
       </c>
-      <c r="AR168" s="59">
+      <c r="AR169" s="59">
+        <v>0</v>
+      </c>
+      <c r="AS169" s="59">
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:44" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B169" s="45"/>
-    </row>
-    <row r="170" spans="1:44" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="54" t="s">
+    <row r="170" spans="1:45" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B170" s="45"/>
+    </row>
+    <row r="171" spans="1:45" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="B170" s="43"/>
-    </row>
-    <row r="171" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="3"/>
-      <c r="B171" s="4"/>
-      <c r="C171" s="3"/>
-      <c r="D171" s="4"/>
-      <c r="E171" s="3"/>
-      <c r="F171" s="4"/>
-      <c r="G171" s="3"/>
-      <c r="H171" s="4"/>
-      <c r="I171" s="4"/>
-      <c r="J171" s="4"/>
-      <c r="K171" s="4"/>
-      <c r="L171" s="4"/>
-      <c r="M171" s="4"/>
-      <c r="N171" s="4"/>
-      <c r="O171" s="4"/>
-      <c r="P171" s="4"/>
-      <c r="Q171" s="4"/>
-      <c r="R171" s="4"/>
-      <c r="S171" s="4"/>
-      <c r="T171" s="4"/>
-      <c r="U171" s="4"/>
-      <c r="V171" s="4"/>
-      <c r="W171" s="4"/>
-      <c r="X171" s="4"/>
-      <c r="Y171" s="4"/>
-      <c r="Z171" s="4"/>
-      <c r="AA171" s="4"/>
-      <c r="AB171" s="4"/>
-      <c r="AC171" s="4"/>
-    </row>
-    <row r="172" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B171" s="43"/>
+    </row>
+    <row r="172" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="3"/>
       <c r="B172" s="4"/>
       <c r="C172" s="3"/>
@@ -8169,7 +8184,7 @@
       <c r="AB172" s="4"/>
       <c r="AC172" s="4"/>
     </row>
-    <row r="173" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3"/>
       <c r="B173" s="4"/>
       <c r="C173" s="3"/>
@@ -8200,7 +8215,7 @@
       <c r="AB173" s="4"/>
       <c r="AC173" s="4"/>
     </row>
-    <row r="174" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="3"/>
       <c r="B174" s="4"/>
       <c r="C174" s="3"/>
@@ -8231,7 +8246,7 @@
       <c r="AB174" s="4"/>
       <c r="AC174" s="4"/>
     </row>
-    <row r="175" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="3"/>
       <c r="B175" s="4"/>
       <c r="C175" s="3"/>
@@ -8262,7 +8277,7 @@
       <c r="AB175" s="4"/>
       <c r="AC175" s="4"/>
     </row>
-    <row r="176" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="3"/>
       <c r="B176" s="4"/>
       <c r="C176" s="3"/>
@@ -34736,6 +34751,37 @@
       <c r="AB1029" s="4"/>
       <c r="AC1029" s="4"/>
     </row>
+    <row r="1030" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1030" s="3"/>
+      <c r="B1030" s="4"/>
+      <c r="C1030" s="3"/>
+      <c r="D1030" s="4"/>
+      <c r="E1030" s="3"/>
+      <c r="F1030" s="4"/>
+      <c r="G1030" s="3"/>
+      <c r="H1030" s="4"/>
+      <c r="I1030" s="4"/>
+      <c r="J1030" s="4"/>
+      <c r="K1030" s="4"/>
+      <c r="L1030" s="4"/>
+      <c r="M1030" s="4"/>
+      <c r="N1030" s="4"/>
+      <c r="O1030" s="4"/>
+      <c r="P1030" s="4"/>
+      <c r="Q1030" s="4"/>
+      <c r="R1030" s="4"/>
+      <c r="S1030" s="4"/>
+      <c r="T1030" s="4"/>
+      <c r="U1030" s="4"/>
+      <c r="V1030" s="4"/>
+      <c r="W1030" s="4"/>
+      <c r="X1030" s="4"/>
+      <c r="Y1030" s="4"/>
+      <c r="Z1030" s="4"/>
+      <c r="AA1030" s="4"/>
+      <c r="AB1030" s="4"/>
+      <c r="AC1030" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C47" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
New note on estimated base-case cost for fuel $/GGE
</commit_message>
<xml_diff>
--- a/Fuels_case_input_test_190827.xlsx
+++ b/Fuels_case_input_test_190827.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/IDrive-Sync/Carnegie/SEM-1.2_CIW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/IDrive-Sync/Carnegie/SEM-1.2_HOME/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA6EF21-FAB7-F846-8051-47F171EAA73F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C879C7-5F13-5243-8DF3-0CCF3C3EBC5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_test_190726" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="215">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -678,6 +678,9 @@
   <si>
     <t>test_190829_v6</t>
   </si>
+  <si>
+    <t>Estimated $/kWh for fuel… FIXME</t>
+  </si>
 </sst>
 </file>
 
@@ -690,7 +693,7 @@
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -728,8 +731,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -808,6 +823,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -829,7 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1024,6 +1045,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1341,12 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5480" ySplit="5320" topLeftCell="A42" activePane="bottomRight"/>
-      <selection activeCell="A62" sqref="A62:XFD62"/>
-      <selection pane="topRight" activeCell="F81" sqref="F81"/>
-      <selection pane="bottomLeft" activeCell="C159" sqref="C159"/>
-      <selection pane="bottomRight" activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7643,6 +7665,16 @@
     <row r="160" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="52"/>
       <c r="B160" s="47"/>
+      <c r="C160" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="D160" s="71">
+        <f>((B149/B155)+(B150+B151+B154+B153))/B156</f>
+        <v>0.18761941388871392</v>
+      </c>
+      <c r="E160" s="72" t="s">
+        <v>96</v>
+      </c>
       <c r="F160" s="8"/>
       <c r="H160" s="8"/>
       <c r="I160" s="3"/>
@@ -7727,7 +7759,6 @@
     </row>
     <row r="163" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3"/>
-      <c r="B163" s="4"/>
       <c r="C163" s="3"/>
       <c r="D163" s="4"/>
       <c r="E163" s="3"/>

</xml_diff>

<commit_message>
Print default system specifications and correct minor 973 --> 971 typo
</commit_message>
<xml_diff>
--- a/Fuels_case_input_test_190827.xlsx
+++ b/Fuels_case_input_test_190827.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/IDrive-Sync/Carnegie/SEM-1.2_HOME/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/SEM-1.2_CIW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C879C7-5F13-5243-8DF3-0CCF3C3EBC5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616C457F-358E-364C-A286-EF1A5516BF71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8520" yWindow="-23080" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_test_190726" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1367,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2835,8 +2837,7 @@
         <v>27</v>
       </c>
       <c r="B46" s="8">
-        <f>(365+1/4-1/100+1/400)*24</f>
-        <v>8765.82</v>
+        <v>8760</v>
       </c>
       <c r="C46" s="9" t="str">
         <f>HYPERLINK("https://en.wikipedia.org/wiki/Leap_year", "Reference: # days per year")</f>
@@ -4124,7 +4125,7 @@
       </c>
       <c r="B81" s="26">
         <f>N81</f>
-        <v>1.9528741509529837E-2</v>
+        <v>1.954171608436836E-2</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>93</v>
@@ -4164,7 +4165,7 @@
       </c>
       <c r="N81" s="29">
         <f>M81/HOURS_PER_YEAR</f>
-        <v>1.9528741509529837E-2</v>
+        <v>1.954171608436836E-2</v>
       </c>
       <c r="O81" s="8"/>
       <c r="P81" s="8"/>
@@ -4400,7 +4401,7 @@
       </c>
       <c r="B87" s="26">
         <f>N87</f>
-        <v>1.9528741509529837E-2</v>
+        <v>1.954171608436836E-2</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>93</v>
@@ -4440,7 +4441,7 @@
       </c>
       <c r="N87" s="29">
         <f>M87/HOURS_PER_YEAR</f>
-        <v>1.9528741509529837E-2</v>
+        <v>1.954171608436836E-2</v>
       </c>
       <c r="O87" s="8"/>
       <c r="P87" s="8"/>
@@ -4676,7 +4677,7 @@
       </c>
       <c r="B93" s="26">
         <f>N93</f>
-        <v>2.0648572594225215E-2</v>
+        <v>2.0662291166428225E-2</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>93</v>
@@ -4716,7 +4717,7 @@
       </c>
       <c r="N93" s="29">
         <f>M93/HOURS_PER_YEAR</f>
-        <v>2.0648572594225215E-2</v>
+        <v>2.0662291166428225E-2</v>
       </c>
       <c r="O93" s="8"/>
       <c r="P93" s="8"/>
@@ -4952,7 +4953,7 @@
       </c>
       <c r="B99" s="26">
         <f>N99</f>
-        <v>2.0648572594225215E-2</v>
+        <v>2.0662291166428225E-2</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>93</v>
@@ -4992,7 +4993,7 @@
       </c>
       <c r="N99" s="29">
         <f>M99/HOURS_PER_YEAR</f>
-        <v>2.0648572594225215E-2</v>
+        <v>2.0662291166428225E-2</v>
       </c>
       <c r="O99" s="8"/>
       <c r="P99" s="8"/>
@@ -5193,7 +5194,7 @@
       </c>
       <c r="B104" s="26">
         <f>N104</f>
-        <v>1.1841887362491711E-2</v>
+        <v>1.1849754917794188E-2</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>93</v>
@@ -5231,7 +5232,7 @@
       </c>
       <c r="N104" s="29">
         <f>M104/HOURS_PER_YEAR</f>
-        <v>1.1841887362491711E-2</v>
+        <v>1.1849754917794188E-2</v>
       </c>
       <c r="O104" s="8"/>
       <c r="P104" s="8"/>
@@ -5433,7 +5434,7 @@
       </c>
       <c r="B109" s="26">
         <f>N109</f>
-        <v>2.7271220888813726E-2</v>
+        <v>2.7289339439678213E-2</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>93</v>
@@ -5471,7 +5472,7 @@
       </c>
       <c r="N109" s="29">
         <f>M109/HOURS_PER_YEAR</f>
-        <v>2.7271220888813726E-2</v>
+        <v>2.7289339439678213E-2</v>
       </c>
       <c r="O109" s="8"/>
       <c r="P109" s="8"/>
@@ -5673,7 +5674,7 @@
       </c>
       <c r="B114" s="26">
         <f>N114</f>
-        <v>6.4753901191501415E-2</v>
+        <v>6.4795381249142345E-2</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>93</v>
@@ -5713,7 +5714,7 @@
       </c>
       <c r="N114" s="36">
         <f>M114/HOURS_PER_YEAR+W115/1000</f>
-        <v>6.4753901191501415E-2</v>
+        <v>6.4795381249142345E-2</v>
       </c>
       <c r="O114" s="8"/>
       <c r="P114" s="8"/>
@@ -5921,7 +5922,7 @@
       </c>
       <c r="B119" s="26">
         <f>N119</f>
-        <v>4.2392529406082022E-3</v>
+        <v>4.2420694305755928E-3</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>128</v>
@@ -5958,7 +5959,7 @@
       </c>
       <c r="N119" s="29">
         <f>M119/HOURS_PER_YEAR</f>
-        <v>4.2392529406082022E-3</v>
+        <v>4.2420694305755928E-3</v>
       </c>
       <c r="O119" s="8"/>
       <c r="P119" s="8"/>
@@ -6127,7 +6128,7 @@
       </c>
       <c r="B123" s="26">
         <f>1.01^(1/HOURS_PER_YEAR)-1</f>
-        <v>1.1351290010175319E-6</v>
+        <v>1.1358831626395727E-6</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>133</v>
@@ -6241,7 +6242,7 @@
       </c>
       <c r="B126" s="26">
         <f>N126</f>
-        <v>4.2392529406082022E-3</v>
+        <v>4.2420694305755928E-3</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>128</v>
@@ -6278,7 +6279,7 @@
       </c>
       <c r="N126" s="29">
         <f>M126/HOURS_PER_YEAR</f>
-        <v>4.2392529406082022E-3</v>
+        <v>4.2420694305755928E-3</v>
       </c>
       <c r="O126" s="8"/>
       <c r="P126" s="8"/>
@@ -6447,7 +6448,7 @@
       </c>
       <c r="B130" s="26">
         <f>1.01^(1/HOURS_PER_YEAR)-1</f>
-        <v>1.1351290010175319E-6</v>
+        <v>1.1358831626395727E-6</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>133</v>
@@ -6561,7 +6562,7 @@
       </c>
       <c r="B133" s="39">
         <f t="shared" ref="B133:B135" si="6">N133</f>
-        <v>3.2304881600325706E-6</v>
+        <v>3.2326344432621811E-6</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>128</v>
@@ -6597,7 +6598,7 @@
       </c>
       <c r="N133" s="41">
         <f>M133/HOURS_PER_YEAR</f>
-        <v>3.2304881600325706E-6</v>
+        <v>3.2326344432621811E-6</v>
       </c>
       <c r="O133" s="8"/>
       <c r="P133" s="8"/>
@@ -6621,7 +6622,7 @@
       </c>
       <c r="B134" s="39">
         <f t="shared" si="6"/>
-        <v>1.184512325345276E-2</v>
+        <v>1.1852992958627998E-2</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>93</v>
@@ -6655,7 +6656,7 @@
       </c>
       <c r="N134" s="29">
         <f>M134/HOURS_PER_YEAR</f>
-        <v>1.184512325345276E-2</v>
+        <v>1.1852992958627998E-2</v>
       </c>
       <c r="O134" s="8"/>
       <c r="P134" s="8"/>
@@ -6679,7 +6680,7 @@
       </c>
       <c r="B135" s="39">
         <f t="shared" si="6"/>
-        <v>4.9534151787166088E-2</v>
+        <v>4.9567061463353448E-2</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>93</v>
@@ -6713,7 +6714,7 @@
       </c>
       <c r="N135" s="29">
         <f>M135/HOURS_PER_YEAR</f>
-        <v>4.9534151787166088E-2</v>
+        <v>4.9567061463353448E-2</v>
       </c>
       <c r="O135" s="8"/>
       <c r="P135" s="8"/>
@@ -6845,7 +6846,7 @@
       </c>
       <c r="B138" s="42">
         <f>1.0001^(1/HOURS_PER_YEAR)-1</f>
-        <v>1.1407375488659E-8</v>
+        <v>1.1414954537158906E-8</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>133</v>
@@ -7211,7 +7212,7 @@
       </c>
       <c r="B149" s="67">
         <f>N149</f>
-        <v>1.430010548488715E-2</v>
+        <v>1.4309606239901081E-2</v>
       </c>
       <c r="C149" s="53" t="s">
         <v>93</v>
@@ -7243,7 +7244,7 @@
       </c>
       <c r="N149" s="41">
         <f>M149/HOURS_PER_YEAR</f>
-        <v>1.430010548488715E-2</v>
+        <v>1.4309606239901081E-2</v>
       </c>
       <c r="O149" s="8"/>
       <c r="P149" s="8"/>
@@ -7264,7 +7265,7 @@
       </c>
       <c r="B150" s="67">
         <f>N150</f>
-        <v>1.6302702492146069E-2</v>
+        <v>1.6313533739692222E-2</v>
       </c>
       <c r="C150" s="53" t="s">
         <v>93</v>
@@ -7296,7 +7297,7 @@
       </c>
       <c r="N150" s="41">
         <f>M150/HOURS_PER_YEAR</f>
-        <v>1.6302702492146069E-2</v>
+        <v>1.6313533739692222E-2</v>
       </c>
       <c r="O150" s="8"/>
       <c r="P150" s="8"/>
@@ -7317,14 +7318,14 @@
       </c>
       <c r="B151" s="67">
         <f>N151</f>
-        <v>2.7204936137143852E-7</v>
+        <v>2.7279082762072303E-7</v>
       </c>
       <c r="C151" s="53" t="s">
         <v>96</v>
       </c>
       <c r="F151" s="8">
-        <f>((33*10^6))/(973*10^9)*1000</f>
-        <v>3.3915724563206573E-2</v>
+        <f>((33*10^6))/(971*10^9)*1000</f>
+        <v>3.3985581874356338E-2</v>
       </c>
       <c r="G151" s="53" t="s">
         <v>202</v>
@@ -7345,11 +7346,11 @@
       <c r="L151" s="4"/>
       <c r="M151" s="28">
         <f t="shared" ref="M151" si="13">F151*J151+K151</f>
-        <v>2.3847357328969834E-3</v>
+        <v>2.3896476499575339E-3</v>
       </c>
       <c r="N151" s="41">
         <f>M151/HOURS_PER_YEAR</f>
-        <v>2.7204936137143852E-7</v>
+        <v>2.7279082762072303E-7</v>
       </c>
       <c r="O151" s="8"/>
       <c r="P151" s="8"/>
@@ -7558,7 +7559,7 @@
       </c>
       <c r="B157" s="49">
         <f>B138</f>
-        <v>1.1407375488659E-8</v>
+        <v>1.1414954537158906E-8</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>133</v>
@@ -7670,7 +7671,7 @@
       </c>
       <c r="D160" s="71">
         <f>((B149/B155)+(B150+B151+B154+B153))/B156</f>
-        <v>0.18761941388871392</v>
+        <v>0.18765715303912431</v>
       </c>
       <c r="E160" s="72" t="s">
         <v>96</v>

</xml_diff>